<commit_message>
Gráfica añadida a PD1
</commit_message>
<xml_diff>
--- a/ut3/PDs/UT03-PD1/UT3-PD1.xlsx
+++ b/ut3/PDs/UT03-PD1/UT3-PD1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federico\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federico\Documents\GitHub\Machine-Learning-Portfolio\ut3\PDs\UT03-PD1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB0742C-EB6C-445E-9CED-2D8DB8519D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20948602-6AE0-4DDC-AF8F-2D63898C2E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{FB04241C-9064-4DAC-8E3B-C220C05D2793}"/>
   </bookViews>
@@ -795,7 +795,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.1877009699145029</c:v>
+                  <c:v>2.1877009699144998</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5593079124464437</c:v>
@@ -4408,7 +4408,7 @@
   <dimension ref="A2:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4554,7 +4554,7 @@
         <v>0.78295000000000003</v>
       </c>
       <c r="G6" s="4">
-        <f t="shared" si="2"/>
+        <f>F6-C6</f>
         <v>-2.21705</v>
       </c>
     </row>
@@ -4577,7 +4577,7 @@
         <v>0.31442300000000001</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" si="3"/>
+        <f>D7+E7*B7</f>
         <v>1.9660584999999999</v>
       </c>
       <c r="G7" s="4">
@@ -5130,7 +5130,7 @@
         <v>6</v>
       </c>
       <c r="E29" s="1">
-        <v>2.1877009699145029</v>
+        <v>2.1877009699144998</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>10</v>

</xml_diff>